<commit_message>
renaming + test repair + final changes
</commit_message>
<xml_diff>
--- a/hrmcore/src/test/resources/header.xlsx
+++ b/hrmcore/src/test/resources/header.xlsx
@@ -360,7 +360,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -378,7 +378,7 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2">
-        <v>1.5</v>
+        <v>74</v>
       </c>
       <c r="B2">
         <v>1.4</v>

</xml_diff>